<commit_message>
sua bao cao tien do
</commit_message>
<xml_diff>
--- a/progress-report/110121209_DuongVanHiep_BaoCaoTienDo.xlsx
+++ b/progress-report/110121209_DuongVanHiep_BaoCaoTienDo.xlsx
@@ -40,7 +40,7 @@
     <t>x</t>
   </si>
   <si>
-    <t>Tìm hiểu Laravel Freamwork</t>
+    <t>Tìm hiểu Laravel Framework</t>
   </si>
   <si>
     <t>Tạo Github Repository</t>
@@ -52,10 +52,10 @@
     <t>laragon (webserver), VS Code (code editor), Git</t>
   </si>
   <si>
-    <t>Khởi tạo dự án bằng TVUSMC với Laravel Freamwork</t>
+    <t>Khởi tạo dự án bằng TVUSMC với Laravel Framework</t>
   </si>
   <si>
-    <t>Thiết kế Database</t>
+    <t>Thiết kế Database, tạo DB Diagram</t>
   </si>
 </sst>
 </file>

</xml_diff>